<commit_message>
Finalizado Wan no Projeto ipv6 Redes
</commit_message>
<xml_diff>
--- a/Redes-IA/Redes/Projeto-P1-ipv6/Matheus_148632_TP2_P1_REDES_2020_2.xlsx
+++ b/Redes-IA/Redes/Projeto-P1-ipv6/Matheus_148632_TP2_P1_REDES_2020_2.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mathw\Documents\Github Projects\Faculdade\Redes-IA\Redes\Projeto-P1-ipv6\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E8C6548-2981-48D6-9AAC-DAE53FF1CF86}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63A9B373-9FCF-4A84-8FDD-D58FB5AD872F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="2340" windowWidth="20730" windowHeight="11310" xr2:uid="{2C35701C-2D34-4D43-813D-D1E50AEE8229}"/>
   </bookViews>
@@ -696,7 +696,102 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -705,105 +800,10 @@
     <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1131,8 +1131,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D1F8E78-1813-4E87-9B9A-52F4EBCC8238}">
   <dimension ref="A1:H43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18:F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1170,7 +1170,7 @@
       <c r="A2" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="42" t="s">
         <v>22</v>
       </c>
       <c r="C2" s="4" t="s">
@@ -1179,10 +1179,10 @@
       <c r="D2" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="39" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1190,197 +1190,197 @@
       <c r="A3" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="B3" s="5"/>
+      <c r="B3" s="42"/>
       <c r="C3" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="E3" s="5"/>
-      <c r="F3" s="6"/>
+      <c r="E3" s="42"/>
+      <c r="F3" s="39"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="B4" s="5"/>
+      <c r="B4" s="42"/>
       <c r="C4" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="E4" s="5"/>
-      <c r="F4" s="6"/>
+      <c r="E4" s="42"/>
+      <c r="F4" s="39"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="F5" s="40" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="7"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="8" t="s">
+      <c r="A6" s="40"/>
+      <c r="B6" s="40"/>
+      <c r="C6" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
+      <c r="E6" s="40"/>
+      <c r="F6" s="40"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="7"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="8" t="s">
+      <c r="A7" s="40"/>
+      <c r="B7" s="40"/>
+      <c r="C7" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
+      <c r="E7" s="40"/>
+      <c r="F7" s="40"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="D8" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
+      <c r="E8" s="40"/>
+      <c r="F8" s="40"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="9"/>
-      <c r="B9" s="9"/>
-      <c r="C9" s="10" t="s">
+      <c r="A9" s="35"/>
+      <c r="B9" s="35"/>
+      <c r="C9" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="D9" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
+      <c r="E9" s="40"/>
+      <c r="F9" s="40"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="7" t="s">
         <v>5</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D10" s="11" t="s">
+      <c r="D10" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="E10" s="12" t="s">
+      <c r="E10" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="F10" s="12" t="s">
+      <c r="F10" s="38" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="12" t="s">
+      <c r="A11" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="12" t="s">
+      <c r="B11" s="38" t="s">
         <v>26</v>
       </c>
-      <c r="C11" s="13" t="s">
+      <c r="C11" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="D11" s="13" t="s">
+      <c r="D11" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
+      <c r="E11" s="38"/>
+      <c r="F11" s="38"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="12"/>
-      <c r="B12" s="12"/>
-      <c r="C12" s="13" t="s">
+      <c r="A12" s="38"/>
+      <c r="B12" s="38"/>
+      <c r="C12" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="D12" s="13" t="s">
+      <c r="D12" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
+      <c r="E12" s="38"/>
+      <c r="F12" s="38"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="12"/>
-      <c r="B13" s="12"/>
-      <c r="C13" s="13" t="s">
+      <c r="A13" s="38"/>
+      <c r="B13" s="38"/>
+      <c r="C13" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="D13" s="13" t="s">
+      <c r="D13" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
+      <c r="E13" s="38"/>
+      <c r="F13" s="38"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="14" t="s">
+      <c r="A14" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="B14" s="14" t="s">
+      <c r="B14" s="41" t="s">
         <v>27</v>
       </c>
-      <c r="C14" s="15" t="s">
+      <c r="C14" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="D14" s="15" t="s">
+      <c r="D14" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
+      <c r="E14" s="38"/>
+      <c r="F14" s="38"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="14"/>
-      <c r="B15" s="14"/>
-      <c r="C15" s="15" t="s">
+      <c r="A15" s="41"/>
+      <c r="B15" s="41"/>
+      <c r="C15" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="D15" s="15" t="s">
+      <c r="D15" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
+      <c r="E15" s="38"/>
+      <c r="F15" s="38"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="16"/>
-      <c r="B16" s="16"/>
-      <c r="C16" s="16"/>
-      <c r="D16" s="16"/>
-      <c r="E16" s="16"/>
-      <c r="F16" s="16"/>
+      <c r="A16" s="10"/>
+      <c r="B16" s="10"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="10"/>
     </row>
     <row r="17" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
@@ -1406,152 +1406,152 @@
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="9" t="s">
+      <c r="A18" s="35" t="s">
         <v>60</v>
       </c>
-      <c r="B18" s="10" t="s">
+      <c r="B18" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="C18" s="17">
+      <c r="C18" s="36">
         <v>2</v>
       </c>
-      <c r="D18" s="17" t="s">
+      <c r="D18" s="36" t="s">
         <v>57</v>
       </c>
-      <c r="E18" s="10" t="s">
+      <c r="E18" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="G18" s="10" t="s">
+      <c r="G18" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="H18" s="10" t="s">
+      <c r="H18" s="6" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="9"/>
-      <c r="B19" s="10" t="s">
+      <c r="A19" s="35"/>
+      <c r="B19" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="C19" s="18"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="10" t="s">
+      <c r="C19" s="37"/>
+      <c r="D19" s="37"/>
+      <c r="E19" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="G19" s="10" t="s">
+      <c r="G19" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="H19" s="10" t="s">
+      <c r="H19" s="6" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="9"/>
-      <c r="B20" s="10" t="s">
+      <c r="A20" s="35"/>
+      <c r="B20" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="C20" s="10">
+      <c r="C20" s="6">
         <v>0</v>
       </c>
-      <c r="D20" s="10" t="s">
+      <c r="D20" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="E20" s="10" t="s">
+      <c r="E20" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="G20" s="10" t="s">
+      <c r="G20" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="H20" s="10" t="s">
+      <c r="H20" s="6" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="19" t="s">
+      <c r="A21" s="32" t="s">
         <v>66</v>
       </c>
-      <c r="B21" s="15" t="s">
+      <c r="B21" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="C21" s="19">
+      <c r="C21" s="32">
         <v>3</v>
       </c>
-      <c r="D21" s="19" t="s">
+      <c r="D21" s="32" t="s">
         <v>57</v>
       </c>
-      <c r="E21" s="15" t="s">
+      <c r="E21" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="G21" s="10" t="s">
+      <c r="G21" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="H21" s="10" t="s">
+      <c r="H21" s="6" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="20"/>
-      <c r="B22" s="15" t="s">
+      <c r="A22" s="34"/>
+      <c r="B22" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="C22" s="21"/>
-      <c r="D22" s="21"/>
-      <c r="E22" s="15" t="s">
+      <c r="C22" s="33"/>
+      <c r="D22" s="33"/>
+      <c r="E22" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="G22" s="15" t="s">
+      <c r="G22" s="9" t="s">
         <v>144</v>
       </c>
-      <c r="H22" s="15" t="s">
+      <c r="H22" s="9" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="21"/>
-      <c r="B23" s="15" t="s">
+      <c r="A23" s="33"/>
+      <c r="B23" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="C23" s="15">
+      <c r="C23" s="9">
         <v>0</v>
       </c>
-      <c r="D23" s="15" t="s">
+      <c r="D23" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="E23" s="15" t="s">
+      <c r="E23" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="G23" s="15" t="s">
+      <c r="G23" s="9" t="s">
         <v>145</v>
       </c>
-      <c r="H23" s="15" t="s">
+      <c r="H23" s="9" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="11" t="s">
+      <c r="A24" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="B24" s="11" t="s">
+      <c r="B24" s="7" t="s">
         <v>160</v>
       </c>
-      <c r="C24" s="11">
+      <c r="C24" s="7">
         <v>0</v>
       </c>
-      <c r="D24" s="11" t="s">
+      <c r="D24" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="E24" s="11" t="s">
+      <c r="E24" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="G24" s="15" t="s">
+      <c r="G24" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="H24" s="15" t="s">
+      <c r="H24" s="9" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="23" t="s">
+      <c r="A25" s="30" t="s">
         <v>78</v>
       </c>
       <c r="B25" s="4" t="s">
@@ -1566,15 +1566,15 @@
       <c r="E25" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="G25" s="11" t="s">
+      <c r="G25" s="7" t="s">
         <v>159</v>
       </c>
-      <c r="H25" s="11" t="s">
+      <c r="H25" s="7" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="24"/>
+      <c r="A26" s="31"/>
       <c r="B26" s="4" t="s">
         <v>81</v>
       </c>
@@ -1595,19 +1595,19 @@
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="22" t="s">
+      <c r="A27" s="11" t="s">
         <v>106</v>
       </c>
-      <c r="B27" s="22" t="s">
+      <c r="B27" s="11" t="s">
         <v>107</v>
       </c>
-      <c r="C27" s="22">
+      <c r="C27" s="11">
         <v>0</v>
       </c>
-      <c r="D27" s="22" t="s">
+      <c r="D27" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="E27" s="22" t="s">
+      <c r="E27" s="11" t="s">
         <v>108</v>
       </c>
       <c r="G27" s="4" t="s">
@@ -1618,35 +1618,35 @@
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="23" t="s">
+      <c r="A28" s="30" t="s">
         <v>109</v>
       </c>
       <c r="B28" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="C28" s="23">
+      <c r="C28" s="30">
         <v>5</v>
       </c>
-      <c r="D28" s="23" t="s">
+      <c r="D28" s="30" t="s">
         <v>57</v>
       </c>
       <c r="E28" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="G28" s="22" t="s">
+      <c r="G28" s="11" t="s">
         <v>149</v>
       </c>
-      <c r="H28" s="22" t="s">
+      <c r="H28" s="11" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="24"/>
+      <c r="A29" s="31"/>
       <c r="B29" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="C29" s="24"/>
-      <c r="D29" s="24"/>
+      <c r="C29" s="31"/>
+      <c r="D29" s="31"/>
       <c r="E29" s="4" t="s">
         <v>113</v>
       </c>
@@ -1658,247 +1658,233 @@
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="25" t="s">
+      <c r="A30" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="B30" s="8" t="s">
+      <c r="B30" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="C30" s="25">
+      <c r="C30" s="24">
         <v>1</v>
       </c>
-      <c r="D30" s="25" t="s">
+      <c r="D30" s="24" t="s">
         <v>57</v>
       </c>
-      <c r="E30" s="8" t="s">
+      <c r="E30" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="G30" s="8" t="s">
+      <c r="G30" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="H30" s="8" t="s">
+      <c r="H30" s="5" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="26"/>
-      <c r="B31" s="8" t="s">
+      <c r="A31" s="25"/>
+      <c r="B31" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="C31" s="26"/>
-      <c r="D31" s="26"/>
-      <c r="E31" s="8" t="s">
+      <c r="C31" s="25"/>
+      <c r="D31" s="25"/>
+      <c r="E31" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="G31" s="8" t="s">
+      <c r="G31" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="H31" s="8" t="s">
+      <c r="H31" s="5" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="26"/>
-      <c r="B32" s="27" t="s">
+      <c r="A32" s="25"/>
+      <c r="B32" s="12" t="s">
         <v>117</v>
       </c>
-      <c r="C32" s="28"/>
-      <c r="D32" s="28"/>
-      <c r="E32" s="8" t="s">
+      <c r="C32" s="26"/>
+      <c r="D32" s="26"/>
+      <c r="E32" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="G32" s="8" t="s">
+      <c r="G32" s="5" t="s">
         <v>153</v>
       </c>
-      <c r="H32" s="8" t="s">
+      <c r="H32" s="5" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="26"/>
-      <c r="B33" s="8" t="s">
+      <c r="A33" s="25"/>
+      <c r="B33" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="C33" s="8">
+      <c r="C33" s="5">
         <v>0</v>
       </c>
-      <c r="D33" s="8" t="s">
+      <c r="D33" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="E33" s="8" t="s">
+      <c r="E33" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="G33" s="8" t="s">
+      <c r="G33" s="5" t="s">
         <v>154</v>
       </c>
-      <c r="H33" s="8" t="s">
+      <c r="H33" s="5" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="29" t="s">
+      <c r="A34" s="27" t="s">
         <v>122</v>
       </c>
-      <c r="B34" s="13" t="s">
+      <c r="B34" s="8" t="s">
         <v>123</v>
       </c>
-      <c r="C34" s="29">
+      <c r="C34" s="27">
         <v>4</v>
       </c>
-      <c r="D34" s="29" t="s">
+      <c r="D34" s="27" t="s">
         <v>57</v>
       </c>
-      <c r="E34" s="13" t="s">
+      <c r="E34" s="8" t="s">
         <v>127</v>
       </c>
-      <c r="G34" s="13" t="s">
+      <c r="G34" s="8" t="s">
         <v>155</v>
       </c>
-      <c r="H34" s="13" t="s">
+      <c r="H34" s="8" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="30"/>
-      <c r="B35" s="13" t="s">
+      <c r="A35" s="28"/>
+      <c r="B35" s="8" t="s">
         <v>124</v>
       </c>
-      <c r="C35" s="30"/>
-      <c r="D35" s="30"/>
-      <c r="E35" s="13" t="s">
+      <c r="C35" s="28"/>
+      <c r="D35" s="28"/>
+      <c r="E35" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="G35" s="13" t="s">
+      <c r="G35" s="8" t="s">
         <v>156</v>
       </c>
-      <c r="H35" s="13" t="s">
+      <c r="H35" s="8" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="30"/>
-      <c r="B36" s="13" t="s">
+      <c r="A36" s="28"/>
+      <c r="B36" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="C36" s="30"/>
-      <c r="D36" s="30"/>
-      <c r="E36" s="13" t="s">
+      <c r="C36" s="28"/>
+      <c r="D36" s="28"/>
+      <c r="E36" s="8" t="s">
         <v>129</v>
       </c>
-      <c r="G36" s="13" t="s">
+      <c r="G36" s="8" t="s">
         <v>157</v>
       </c>
-      <c r="H36" s="13" t="s">
+      <c r="H36" s="8" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="31"/>
-      <c r="B37" s="13" t="s">
+      <c r="A37" s="29"/>
+      <c r="B37" s="8" t="s">
         <v>125</v>
       </c>
-      <c r="C37" s="31"/>
-      <c r="D37" s="31"/>
-      <c r="E37" s="13" t="s">
+      <c r="C37" s="29"/>
+      <c r="D37" s="29"/>
+      <c r="E37" s="8" t="s">
         <v>130</v>
       </c>
-      <c r="G37" s="13" t="s">
+      <c r="G37" s="8" t="s">
         <v>158</v>
       </c>
-      <c r="H37" s="13" t="s">
+      <c r="H37" s="8" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="32" t="s">
+      <c r="A38" s="15" t="s">
         <v>131</v>
       </c>
-      <c r="B38" s="33" t="s">
+      <c r="B38" s="13" t="s">
         <v>138</v>
       </c>
-      <c r="C38" s="34">
+      <c r="C38" s="18">
         <v>0</v>
       </c>
-      <c r="D38" s="35" t="s">
+      <c r="D38" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="E38" s="36" t="s">
+      <c r="E38" s="14" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="37"/>
-      <c r="B39" s="33" t="s">
+      <c r="A39" s="16"/>
+      <c r="B39" s="13" t="s">
         <v>139</v>
       </c>
-      <c r="C39" s="38"/>
-      <c r="D39" s="39"/>
-      <c r="E39" s="36" t="s">
+      <c r="C39" s="19"/>
+      <c r="D39" s="22"/>
+      <c r="E39" s="14" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="37"/>
-      <c r="B40" s="33" t="s">
+      <c r="A40" s="16"/>
+      <c r="B40" s="13" t="s">
         <v>140</v>
       </c>
-      <c r="C40" s="38"/>
-      <c r="D40" s="39"/>
-      <c r="E40" s="36" t="s">
+      <c r="C40" s="19"/>
+      <c r="D40" s="22"/>
+      <c r="E40" s="14" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" s="37"/>
-      <c r="B41" s="33" t="s">
+      <c r="A41" s="16"/>
+      <c r="B41" s="13" t="s">
         <v>141</v>
       </c>
-      <c r="C41" s="38"/>
-      <c r="D41" s="39"/>
-      <c r="E41" s="36" t="s">
+      <c r="C41" s="19"/>
+      <c r="D41" s="22"/>
+      <c r="E41" s="14" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" s="37"/>
-      <c r="B42" s="33" t="s">
+      <c r="A42" s="16"/>
+      <c r="B42" s="13" t="s">
         <v>142</v>
       </c>
-      <c r="C42" s="38"/>
-      <c r="D42" s="39"/>
-      <c r="E42" s="36" t="s">
+      <c r="C42" s="19"/>
+      <c r="D42" s="22"/>
+      <c r="E42" s="14" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A43" s="40"/>
-      <c r="B43" s="33" t="s">
+      <c r="A43" s="17"/>
+      <c r="B43" s="13" t="s">
         <v>143</v>
       </c>
-      <c r="C43" s="41"/>
-      <c r="D43" s="42"/>
-      <c r="E43" s="36" t="s">
+      <c r="C43" s="20"/>
+      <c r="D43" s="23"/>
+      <c r="E43" s="14" t="s">
         <v>137</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="A38:A43"/>
-    <mergeCell ref="C38:C43"/>
-    <mergeCell ref="D38:D43"/>
-    <mergeCell ref="C30:C32"/>
-    <mergeCell ref="D30:D32"/>
-    <mergeCell ref="A30:A33"/>
-    <mergeCell ref="A34:A37"/>
-    <mergeCell ref="C34:C37"/>
-    <mergeCell ref="D34:D37"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="D28:D29"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="A21:A23"/>
-    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="B8:B9"/>
     <mergeCell ref="A18:A20"/>
     <mergeCell ref="D18:D19"/>
     <mergeCell ref="C18:C19"/>
@@ -1915,8 +1901,22 @@
     <mergeCell ref="B2:B4"/>
     <mergeCell ref="A5:A7"/>
     <mergeCell ref="B5:B7"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="A21:A23"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="A38:A43"/>
+    <mergeCell ref="C38:C43"/>
+    <mergeCell ref="D38:D43"/>
+    <mergeCell ref="C30:C32"/>
+    <mergeCell ref="D30:D32"/>
+    <mergeCell ref="A30:A33"/>
+    <mergeCell ref="A34:A37"/>
+    <mergeCell ref="C34:C37"/>
+    <mergeCell ref="D34:D37"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>